<commit_message>
added files in the list
</commit_message>
<xml_diff>
--- a/mediaquery.xlsx
+++ b/mediaquery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Development\KodeGoRemedialClass\Section1Mp3Player\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6072C666-55CF-4F24-AE88-EBF2978BBA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C559DD5-9469-4DA6-9F04-F1E2AA909655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{8E55C6A9-1D91-4BD4-BECE-6F6AFCD98D46}"/>
   </bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A5:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>